<commit_message>
kế hoạch thực hiện
</commit_message>
<xml_diff>
--- a/Project_plan.xlsx
+++ b/Project_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HCMUS\23-24 HK1\Nhap_mon_CNTT(TH)\PROJECT\DETECT_NUMBER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65503083-31DB-47D9-A4FA-DE561B326BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7F5061-AE86-4A94-8787-50760BD2E261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78CCAFD8-AE9B-4DD7-81F5-10F14805280D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN ĐỒ ÁN NHẬP MÔN CÔNG NGHỆ THÔNG TIN</t>
   </si>
@@ -320,6 +320,10 @@
   </si>
   <si>
     <t>Mở team hoặc họp offline để xem kết quả của nhóm</t>
+  </si>
+  <si>
+    <t>Võ Hàn Trân Châu
+Huỳnh Quốc Huy</t>
   </si>
 </sst>
 </file>
@@ -739,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -763,7 +767,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -779,7 +782,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -805,16 +807,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -840,12 +839,25 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -864,41 +876,35 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1217,7 +1223,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="E9" sqref="E9:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,29 +1233,29 @@
     <col min="3" max="3" width="39.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="74.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="39" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="34" customWidth="1"/>
     <col min="7" max="7" width="23" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4"/>
@@ -1259,13 +1265,13 @@
       <c r="C3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="33"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4"/>
@@ -1275,13 +1281,13 @@
       <c r="C4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>43</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="34"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4"/>
@@ -1291,608 +1297,614 @@
       <c r="C5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E5" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="35"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="58" t="s">
+      <c r="G7" s="43" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="44"/>
+      <c r="B8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="59"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="44"/>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="63">
+      <c r="A9" s="55">
         <v>1</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="14" t="s">
+      <c r="A10" s="56"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="64"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="14" t="s">
+      <c r="A11" s="56"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="14" t="s">
+    <row r="12" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="56"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="25" t="s">
-        <v>34</v>
+      <c r="G12" s="59" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="14" t="s">
+      <c r="A13" s="56"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="65"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="43" t="s">
+      <c r="A14" s="57"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="51">
+      <c r="A15" s="49">
         <v>2</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="26" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="14" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>63</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="14" t="s">
+      <c r="A17" s="50"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="14" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>57</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="F18" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G18" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="14" t="s">
+    <row r="19" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="50"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="38" t="s">
+      <c r="F19" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="G19" s="25" t="s">
-        <v>34</v>
+      <c r="G19" s="59" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="14" t="s">
+      <c r="A20" s="50"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="53"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="26" t="s">
+      <c r="A21" s="51"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="52">
+      <c r="A22" s="50">
         <v>3</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="47" t="s">
+      <c r="G22" s="40" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="14" t="s">
+      <c r="A23" s="50"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>57</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="38" t="s">
+      <c r="F23" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="14" t="s">
+    <row r="24" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="50"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="38" t="s">
+      <c r="F24" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="25" t="s">
-        <v>34</v>
+      <c r="G24" s="59" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="14" t="s">
+      <c r="A25" s="50"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="38" t="s">
+      <c r="F25" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="24" t="s">
+      <c r="G25" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="52"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="43" t="s">
+      <c r="A26" s="50"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="41" t="s">
+      <c r="F26" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="42" t="s">
+      <c r="G26" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="51">
+      <c r="A27" s="49">
         <v>4</v>
       </c>
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="45" t="s">
+      <c r="D27" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F27" s="36" t="s">
+      <c r="F27" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="14" t="s">
+      <c r="A28" s="50"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="8" t="s">
         <v>57</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="38" t="s">
+      <c r="F28" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="24" t="s">
+      <c r="G28" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="14" t="s">
+    <row r="29" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="50"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="38" t="s">
+      <c r="F29" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="G29" s="25" t="s">
-        <v>34</v>
+      <c r="G29" s="59" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="14" t="s">
+      <c r="A30" s="50"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="38" t="s">
+      <c r="F30" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="G30" s="24" t="s">
+      <c r="G30" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="52"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="43" t="s">
+      <c r="A31" s="50"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="E31" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="F31" s="41" t="s">
+      <c r="F31" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="G31" s="42" t="s">
+      <c r="G31" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="51">
+      <c r="A32" s="49">
         <v>5</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="F32" s="36" t="s">
+      <c r="F32" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G32" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="14" t="s">
+      <c r="A33" s="50"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="8" t="s">
         <v>95</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F33" s="38" t="s">
+      <c r="F33" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="G33" s="23" t="s">
+      <c r="G33" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="14" t="s">
+    <row r="34" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="50"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="38" t="s">
+      <c r="F34" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="25" t="s">
-        <v>34</v>
+      <c r="G34" s="59" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="14" t="s">
+      <c r="A35" s="50"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F35" s="38" t="s">
+      <c r="F35" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="G35" s="24" t="s">
+      <c r="G35" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="53"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="26" t="s">
+      <c r="A36" s="51"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="32" t="s">
+      <c r="F36" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="G36" s="29" t="s">
+      <c r="G36" s="25" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="A27:A31"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="A1:G2"/>
@@ -1905,12 +1917,6 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="A27:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix plan for 2nd week
</commit_message>
<xml_diff>
--- a/Project_plan.xlsx
+++ b/Project_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HCMUS\23-24 HK1\Nhap_mon_CNTT(TH)\PROJECT\DETECT_NUMBER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17916FBB-1255-447F-B06E-5142240E91B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E635FA8-ABEF-4D3F-BE14-4BB3F65D7073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78CCAFD8-AE9B-4DD7-81F5-10F14805280D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="97">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN ĐỒ ÁN NHẬP MÔN CÔNG NGHỆ THÔNG TIN</t>
   </si>
@@ -193,12 +193,6 @@
     <t>Viết code tổng hợp lại 3 file cài đặt ở trên</t>
   </si>
   <si>
-    <t>02/12</t>
-  </si>
-  <si>
-    <t>30/11</t>
-  </si>
-  <si>
     <t>Cài đặt bộ phân lớp kNN</t>
   </si>
   <si>
@@ -257,9 +251,6 @@
   </si>
   <si>
     <t>11/12</t>
-  </si>
-  <si>
-    <t>04/12</t>
   </si>
   <si>
     <t>27/11</t>
@@ -329,7 +320,13 @@
     <t>Tổng hợp vào file main.py in ra màng hình để quay demo và nộp bài</t>
   </si>
   <si>
-    <t>01/11</t>
+    <t>05/12</t>
+  </si>
+  <si>
+    <t>04/11</t>
+  </si>
+  <si>
+    <t>03/11</t>
   </si>
 </sst>
 </file>
@@ -749,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -821,31 +818,19 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -858,6 +843,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -873,33 +882,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -909,8 +897,26 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1228,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F2594A-11CA-4C50-84CA-0D38651FB73F}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,7 +1245,7 @@
     <col min="3" max="3" width="39.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="74.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="60" customWidth="1"/>
     <col min="7" max="7" width="23" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1277,7 +1283,7 @@
       <c r="E3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="28"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4"/>
@@ -1291,9 +1297,9 @@
         <v>43</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="29"/>
+        <v>82</v>
+      </c>
+      <c r="F4" s="54"/>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4"/>
@@ -1306,16 +1312,16 @@
       <c r="D5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="30"/>
+      <c r="E5" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="55"/>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="30"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="55"/>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
@@ -1352,10 +1358,10 @@
       <c r="G8" s="47"/>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="58">
+      <c r="A9" s="51">
         <v>1</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="17" t="s">
@@ -1367,7 +1373,7 @@
       <c r="E9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="56" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="20" t="s">
@@ -1375,8 +1381,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
@@ -1386,7 +1392,7 @@
       <c r="E10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="28" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="21" t="s">
@@ -1394,8 +1400,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="13" t="s">
         <v>9</v>
       </c>
@@ -1405,7 +1411,7 @@
       <c r="E11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="28" t="s">
         <v>29</v>
       </c>
       <c r="G11" s="22" t="s">
@@ -1413,8 +1419,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="13" t="s">
         <v>10</v>
       </c>
@@ -1424,16 +1430,16 @@
       <c r="E12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="41" t="s">
-        <v>92</v>
+      <c r="G12" s="33" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="50"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
@@ -1443,7 +1449,7 @@
       <c r="E13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="28" t="s">
         <v>30</v>
       </c>
       <c r="G13" s="22" t="s">
@@ -1451,69 +1457,69 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="60"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="38" t="s">
+      <c r="A14" s="53"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="37" t="s">
+      <c r="F14" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="52">
+      <c r="A15" s="39">
         <v>2</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="36" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>47</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>56</v>
+        <v>90</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>96</v>
       </c>
       <c r="G15" s="26" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="13" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>56</v>
+        <v>91</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>96</v>
       </c>
       <c r="G16" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="13" t="s">
         <v>49</v>
       </c>
@@ -1521,18 +1527,18 @@
         <v>50</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>56</v>
+        <v>92</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>96</v>
       </c>
       <c r="G17" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="50"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="13" t="s">
         <v>53</v>
       </c>
@@ -1540,18 +1546,18 @@
         <v>54</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>97</v>
+        <v>93</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>95</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="50"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="13" t="s">
         <v>10</v>
       </c>
@@ -1561,16 +1567,16 @@
       <c r="E19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="41" t="s">
+      <c r="F19" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="33" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="13" t="s">
         <v>11</v>
       </c>
@@ -1578,18 +1584,18 @@
         <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>55</v>
+        <v>77</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>94</v>
       </c>
       <c r="G20" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="51"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="23" t="s">
         <v>12</v>
       </c>
@@ -1597,41 +1603,41 @@
         <v>19</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>94</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="53">
+      <c r="A22" s="40">
         <v>3</v>
       </c>
-      <c r="B22" s="61" t="s">
-        <v>57</v>
+      <c r="B22" s="42" t="s">
+        <v>55</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>60</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="32" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="13" t="s">
         <v>53</v>
       </c>
@@ -1639,18 +1645,18 @@
         <v>54</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="33" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>59</v>
       </c>
       <c r="G23" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="13" t="s">
         <v>10</v>
       </c>
@@ -1660,16 +1666,16 @@
       <c r="E24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24" s="41" t="s">
-        <v>92</v>
+      <c r="F24" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="13" t="s">
         <v>11</v>
       </c>
@@ -1677,60 +1683,60 @@
         <v>18</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>61</v>
+        <v>78</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>59</v>
       </c>
       <c r="G25" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="53"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="38" t="s">
+      <c r="A26" s="40"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="F26" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="G26" s="37" t="s">
+      <c r="E26" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="52">
+      <c r="A27" s="39">
         <v>4</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="43" t="s">
+      <c r="F27" s="56" t="s">
         <v>66</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="31" t="s">
-        <v>68</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
-      <c r="B28" s="50"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="13" t="s">
         <v>53</v>
       </c>
@@ -1738,18 +1744,18 @@
         <v>54</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>67</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="50"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="13" t="s">
         <v>10</v>
       </c>
@@ -1759,16 +1765,16 @@
       <c r="E29" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="G29" s="41" t="s">
-        <v>92</v>
+      <c r="F29" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
-      <c r="B30" s="50"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="13" t="s">
         <v>11</v>
       </c>
@@ -1778,77 +1784,77 @@
       <c r="E30" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="33" t="s">
-        <v>69</v>
+      <c r="F30" s="28" t="s">
+        <v>67</v>
       </c>
       <c r="G30" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="53"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="38" t="s">
+      <c r="A31" s="40"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F31" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="G31" s="37" t="s">
+      <c r="F31" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="52">
+      <c r="A32" s="39">
         <v>5</v>
       </c>
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>72</v>
-      </c>
       <c r="D32" s="18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F32" s="31" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="F32" s="56" t="s">
+        <v>84</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
-      <c r="B33" s="50"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="37"/>
       <c r="C33" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F33" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="F33" s="28" t="s">
+        <v>84</v>
       </c>
       <c r="G33" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
-      <c r="B34" s="50"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="37"/>
       <c r="C34" s="13" t="s">
         <v>10</v>
       </c>
@@ -1858,16 +1864,16 @@
       <c r="E34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="G34" s="41" t="s">
-        <v>92</v>
+      <c r="F34" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
-      <c r="B35" s="50"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="37"/>
       <c r="C35" s="13" t="s">
         <v>11</v>
       </c>
@@ -1875,18 +1881,18 @@
         <v>18</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F35" s="33" t="s">
-        <v>73</v>
+        <v>80</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>71</v>
       </c>
       <c r="G35" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="54"/>
-      <c r="B36" s="51"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="23" t="s">
         <v>12</v>
       </c>
@@ -1894,10 +1900,10 @@
         <v>19</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>74</v>
+        <v>81</v>
+      </c>
+      <c r="F36" s="58" t="s">
+        <v>72</v>
       </c>
       <c r="G36" s="25" t="s">
         <v>33</v>
@@ -1905,12 +1911,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="A27:A31"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="A1:G2"/>
@@ -1923,6 +1923,12 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="A27:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>